<commit_message>
Chien luoc giao dich cap XAUUSD
</commit_message>
<xml_diff>
--- a/Indicator/Bollinger band/XAUUSD.xlsx
+++ b/Indicator/Bollinger band/XAUUSD.xlsx
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A283" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I299" sqref="I299"/>
+    <sheetView tabSelected="1" topLeftCell="A289" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q304" sqref="Q304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>